<commit_message>
Added ability to remove channels and change channel removal flags.
</commit_message>
<xml_diff>
--- a/sample_files/Raw Boreholes/LS-27-21-07/RAW/DDH-LS-27-21-07-in.xlsx
+++ b/sample_files/Raw Boreholes/LS-27-21-07/RAW/DDH-LS-27-21-07-in.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irene\Desktop\1. IZCAYCRUZ 2021\8. MEDICIONES GYRO\NIVEL 27\03-07-2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irene\Desktop\1. IZCAYCRUZ 2021\8. MEDICIONES GYRO\NIVEL 27\06-07-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16351895-0C27-4CCA-A2AD-7014D39C4E2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D5AA021-0404-40FD-AAE3-155A6E7860E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
@@ -380,7 +380,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,16 +563,16 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -929,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1004,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2">
-        <v>-85.624399999999994</v>
+        <v>-85.549300000000002</v>
       </c>
       <c r="C4" s="2">
         <v>289.23899999999998</v>
@@ -1027,22 +1027,22 @@
         <v>10</v>
       </c>
       <c r="B5" s="2">
-        <v>-85.512900000000002</v>
+        <v>-85.378</v>
       </c>
       <c r="C5" s="2">
-        <v>288.89339999999999</v>
+        <v>288.39999999999998</v>
       </c>
       <c r="D5" s="2">
-        <v>0.34399999999999997</v>
+        <v>0.55120000000000002</v>
       </c>
       <c r="E5" s="2">
-        <v>311341.1997</v>
+        <v>311341.1814</v>
       </c>
       <c r="F5" s="2">
-        <v>8807893.4724000003</v>
+        <v>8807893.4749999996</v>
       </c>
       <c r="G5" s="2">
-        <v>4183.0699000000004</v>
+        <v>4183.0712999999996</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1050,22 +1050,22 @@
         <v>20</v>
       </c>
       <c r="B6" s="2">
-        <v>-85.423000000000002</v>
+        <v>-85.495500000000007</v>
       </c>
       <c r="C6" s="2">
-        <v>287.56970000000001</v>
+        <v>285.8587</v>
       </c>
       <c r="D6" s="2">
-        <v>0.4138</v>
+        <v>0.70150000000000001</v>
       </c>
       <c r="E6" s="2">
-        <v>311340.44919999997</v>
+        <v>311340.42129999999</v>
       </c>
       <c r="F6" s="2">
-        <v>8807893.7194999997</v>
+        <v>8807893.7094999999</v>
       </c>
       <c r="G6" s="2">
-        <v>4173.1012000000001</v>
+        <v>4173.1030000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1073,22 +1073,22 @@
         <v>30</v>
       </c>
       <c r="B7" s="2">
-        <v>-85.533199999999994</v>
+        <v>-85.518799999999999</v>
       </c>
       <c r="C7" s="2">
-        <v>286.07819999999998</v>
+        <v>286.8546</v>
       </c>
       <c r="D7" s="2">
-        <v>0.48349999999999999</v>
+        <v>0.2442</v>
       </c>
       <c r="E7" s="2">
-        <v>311339.69469999999</v>
+        <v>311339.66970000003</v>
       </c>
       <c r="F7" s="2">
-        <v>8807893.9477999993</v>
+        <v>8807893.9300999995</v>
       </c>
       <c r="G7" s="2">
-        <v>4163.1323000000002</v>
+        <v>4163.1337999999996</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1096,22 +1096,22 @@
         <v>40</v>
       </c>
       <c r="B8" s="2">
-        <v>-85.677499999999995</v>
+        <v>-85.644099999999995</v>
       </c>
       <c r="C8" s="2">
-        <v>284.72680000000003</v>
+        <v>286.85739999999998</v>
       </c>
       <c r="D8" s="2">
-        <v>0.53280000000000005</v>
+        <v>0.376</v>
       </c>
       <c r="E8" s="2">
-        <v>311338.95600000001</v>
+        <v>311338.93239999999</v>
       </c>
       <c r="F8" s="2">
-        <v>8807894.1513999999</v>
+        <v>8807894.1535</v>
       </c>
       <c r="G8" s="2">
-        <v>4153.1616999999997</v>
+        <v>4153.1634999999997</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1119,22 +1119,22 @@
         <v>50</v>
       </c>
       <c r="B9" s="2">
-        <v>-85.665000000000006</v>
+        <v>-85.622900000000001</v>
       </c>
       <c r="C9" s="2">
-        <v>286.7371</v>
+        <v>285.85480000000001</v>
       </c>
       <c r="D9" s="2">
-        <v>0.45669999999999999</v>
+        <v>0.23760000000000001</v>
       </c>
       <c r="E9" s="2">
-        <v>311338.22960000002</v>
+        <v>311338.20179999998</v>
       </c>
       <c r="F9" s="2">
-        <v>8807894.3561000004</v>
+        <v>8807894.3679000009</v>
       </c>
       <c r="G9" s="2">
-        <v>4143.1902</v>
+        <v>4143.1925000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1142,22 +1142,22 @@
         <v>60</v>
       </c>
       <c r="B10" s="2">
-        <v>-85.660600000000002</v>
+        <v>-85.6875</v>
       </c>
       <c r="C10" s="2">
-        <v>283.60000000000002</v>
+        <v>284.66500000000002</v>
       </c>
       <c r="D10" s="2">
-        <v>0.71179999999999999</v>
+        <v>0.3327</v>
       </c>
       <c r="E10" s="2">
-        <v>311337.5</v>
+        <v>311337.47100000002</v>
       </c>
       <c r="F10" s="2">
-        <v>8807894.5538999997</v>
+        <v>8807894.5672999993</v>
       </c>
       <c r="G10" s="2">
-        <v>4133.2188999999998</v>
+        <v>4133.2213000000002</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1165,22 +1165,22 @@
         <v>70</v>
       </c>
       <c r="B11" s="2">
-        <v>-85.673299999999998</v>
+        <v>-85.6584</v>
       </c>
       <c r="C11" s="2">
-        <v>284.86079999999998</v>
+        <v>285.77440000000001</v>
       </c>
       <c r="D11" s="2">
-        <v>0.2883</v>
+        <v>0.26590000000000003</v>
       </c>
       <c r="E11" s="2">
-        <v>311336.76770000003</v>
+        <v>311336.74300000002</v>
       </c>
       <c r="F11" s="2">
-        <v>8807894.7396000009</v>
+        <v>8807894.7653999999</v>
       </c>
       <c r="G11" s="2">
-        <v>4123.2475000000004</v>
+        <v>4123.2497999999996</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1188,22 +1188,22 @@
         <v>80</v>
       </c>
       <c r="B12" s="2">
-        <v>-85.581900000000005</v>
+        <v>-85.529700000000005</v>
       </c>
       <c r="C12" s="2">
-        <v>285.61270000000002</v>
+        <v>284.38900000000001</v>
       </c>
       <c r="D12" s="2">
-        <v>0.3236</v>
+        <v>0.50090000000000001</v>
       </c>
       <c r="E12" s="2">
-        <v>311336.03210000001</v>
+        <v>311336.0013</v>
       </c>
       <c r="F12" s="2">
-        <v>8807894.9399999995</v>
+        <v>8807894.9650999997</v>
       </c>
       <c r="G12" s="2">
-        <v>4113.2766000000001</v>
+        <v>4113.2793000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1211,22 +1211,22 @@
         <v>90</v>
       </c>
       <c r="B13" s="2">
-        <v>-85.644300000000001</v>
+        <v>-85.561999999999998</v>
       </c>
       <c r="C13" s="2">
-        <v>284.92910000000001</v>
+        <v>284.78280000000001</v>
       </c>
       <c r="D13" s="2">
-        <v>0.2442</v>
+        <v>0.13339999999999999</v>
       </c>
       <c r="E13" s="2">
-        <v>311335.2942</v>
+        <v>311335.24969999999</v>
       </c>
       <c r="F13" s="2">
-        <v>8807895.1414999999</v>
+        <v>8807895.1607000008</v>
       </c>
       <c r="G13" s="2">
-        <v>4103.3059000000003</v>
+        <v>4103.3095000000003</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1234,22 +1234,22 @@
         <v>100</v>
       </c>
       <c r="B14" s="2">
-        <v>-85.671199999999999</v>
+        <v>-85.558999999999997</v>
       </c>
       <c r="C14" s="2">
-        <v>286.00189999999998</v>
+        <v>285.92529999999999</v>
       </c>
       <c r="D14" s="2">
-        <v>0.25669999999999998</v>
+        <v>0.26550000000000001</v>
       </c>
       <c r="E14" s="2">
-        <v>311334.56449999998</v>
+        <v>311334.50329999998</v>
       </c>
       <c r="F14" s="2">
-        <v>8807895.3432999998</v>
+        <v>8807895.3657000009</v>
       </c>
       <c r="G14" s="2">
-        <v>4093.3346000000001</v>
+        <v>4093.3395</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1257,22 +1257,22 @@
         <v>110</v>
       </c>
       <c r="B15" s="2">
-        <v>-85.595399999999998</v>
+        <v>-85.602900000000005</v>
       </c>
       <c r="C15" s="2">
-        <v>285.3098</v>
+        <v>287.4984</v>
       </c>
       <c r="D15" s="2">
-        <v>0.27689999999999998</v>
+        <v>0.38669999999999999</v>
       </c>
       <c r="E15" s="2">
-        <v>311333.83140000002</v>
+        <v>311333.76539999997</v>
       </c>
       <c r="F15" s="2">
-        <v>8807895.5488000009</v>
+        <v>8807895.5870999992</v>
       </c>
       <c r="G15" s="2">
-        <v>4083.3636000000001</v>
+        <v>4083.3692999999998</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1280,22 +1280,22 @@
         <v>120</v>
       </c>
       <c r="B16" s="2">
-        <v>-85.783500000000004</v>
+        <v>-85.619799999999998</v>
       </c>
       <c r="C16" s="2">
-        <v>286.04950000000002</v>
+        <v>286.0283</v>
       </c>
       <c r="D16" s="2">
-        <v>0.58850000000000002</v>
+        <v>0.3412</v>
       </c>
       <c r="E16" s="2">
-        <v>311333.10769999999</v>
+        <v>311333.03279999999</v>
       </c>
       <c r="F16" s="2">
-        <v>8807895.7518000007</v>
+        <v>8807895.8079000004</v>
       </c>
       <c r="G16" s="2">
-        <v>4073.3919000000001</v>
+        <v>4073.3986</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1303,22 +1303,22 @@
         <v>130</v>
       </c>
       <c r="B17" s="2">
-        <v>-85.698599999999999</v>
+        <v>-85.607799999999997</v>
       </c>
       <c r="C17" s="2">
-        <v>286.01119999999997</v>
+        <v>286.5129</v>
       </c>
       <c r="D17" s="2">
-        <v>0.25480000000000003</v>
+        <v>0.1168</v>
       </c>
       <c r="E17" s="2">
-        <v>311332.39399999997</v>
+        <v>311332.29859999998</v>
       </c>
       <c r="F17" s="2">
-        <v>8807895.9569000006</v>
+        <v>8807896.0220999997</v>
       </c>
       <c r="G17" s="2">
-        <v>4063.4195</v>
+        <v>4063.4279000000001</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1326,22 +1326,22 @@
         <v>140</v>
       </c>
       <c r="B18" s="2">
-        <v>-85.732699999999994</v>
+        <v>-85.680400000000006</v>
       </c>
       <c r="C18" s="2">
-        <v>286.87909999999999</v>
+        <v>288.20389999999998</v>
       </c>
       <c r="D18" s="2">
-        <v>0.21970000000000001</v>
+        <v>0.4425</v>
       </c>
       <c r="E18" s="2">
-        <v>311331.67749999999</v>
+        <v>311331.57380000001</v>
       </c>
       <c r="F18" s="2">
-        <v>8807896.1682999991</v>
+        <v>8807896.2486000005</v>
       </c>
       <c r="G18" s="2">
-        <v>4053.4475000000002</v>
+        <v>4053.4567999999999</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1349,22 +1349,22 @@
         <v>150</v>
       </c>
       <c r="B19" s="2">
-        <v>-85.760800000000003</v>
+        <v>-85.784400000000005</v>
       </c>
       <c r="C19" s="2">
-        <v>286.62709999999998</v>
+        <v>288.5206</v>
       </c>
       <c r="D19" s="2">
-        <v>0.1014</v>
+        <v>0.31990000000000002</v>
       </c>
       <c r="E19" s="2">
-        <v>311330.96730000002</v>
+        <v>311330.86749999999</v>
       </c>
       <c r="F19" s="2">
-        <v>8807896.3820999991</v>
+        <v>8807896.4829999991</v>
       </c>
       <c r="G19" s="2">
-        <v>4043.4749999999999</v>
+        <v>4043.4845</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1372,22 +1372,22 @@
         <v>160</v>
       </c>
       <c r="B20" s="2">
-        <v>-85.477199999999996</v>
+        <v>-85.492400000000004</v>
       </c>
       <c r="C20" s="2">
-        <v>286.21589999999998</v>
+        <v>287.42200000000003</v>
       </c>
       <c r="D20" s="2">
-        <v>0.85599999999999998</v>
+        <v>0.91120000000000001</v>
       </c>
       <c r="E20" s="2">
-        <v>311330.23460000003</v>
+        <v>311330.14399999997</v>
       </c>
       <c r="F20" s="2">
-        <v>8807896.5979999993</v>
+        <v>8807896.7173999995</v>
       </c>
       <c r="G20" s="2">
-        <v>4033.5043000000001</v>
+        <v>4033.5135</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1395,22 +1395,22 @@
         <v>170</v>
       </c>
       <c r="B21" s="2">
-        <v>-85.508600000000001</v>
+        <v>-85.493600000000001</v>
       </c>
       <c r="C21" s="2">
-        <v>285.47859999999997</v>
+        <v>286.93689999999998</v>
       </c>
       <c r="D21" s="2">
-        <v>0.1976</v>
+        <v>0.1144</v>
       </c>
       <c r="E21" s="2">
-        <v>311329.47859999997</v>
+        <v>311329.3933</v>
       </c>
       <c r="F21" s="2">
-        <v>8807896.8125999998</v>
+        <v>8807896.9495000001</v>
       </c>
       <c r="G21" s="2">
-        <v>4023.5351999999998</v>
+        <v>4023.5444000000002</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1418,22 +1418,22 @@
         <v>180</v>
       </c>
       <c r="B22" s="2">
-        <v>-85.390100000000004</v>
+        <v>-85.530699999999996</v>
       </c>
       <c r="C22" s="2">
-        <v>284.90649999999999</v>
+        <v>286.97840000000002</v>
       </c>
       <c r="D22" s="2">
-        <v>0.38069999999999998</v>
+        <v>0.1118</v>
       </c>
       <c r="E22" s="2">
-        <v>311328.71289999998</v>
+        <v>311328.64480000001</v>
       </c>
       <c r="F22" s="2">
-        <v>8807897.0204000007</v>
+        <v>8807897.1776999999</v>
       </c>
       <c r="G22" s="2">
-        <v>4013.5666999999999</v>
+        <v>4013.5751</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1441,22 +1441,22 @@
         <v>190</v>
       </c>
       <c r="B23" s="2">
-        <v>-85.428799999999995</v>
+        <v>-85.406400000000005</v>
       </c>
       <c r="C23" s="2">
-        <v>286.4547</v>
+        <v>287.31880000000001</v>
       </c>
       <c r="D23" s="2">
-        <v>0.38950000000000001</v>
+        <v>0.38140000000000002</v>
       </c>
       <c r="E23" s="2">
-        <v>311327.9424</v>
+        <v>311327.88990000001</v>
       </c>
       <c r="F23" s="2">
-        <v>8807897.2367000002</v>
+        <v>8807897.4107000008</v>
       </c>
       <c r="G23" s="2">
-        <v>4003.5988000000002</v>
+        <v>4003.6062999999999</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1464,22 +1464,22 @@
         <v>200</v>
       </c>
       <c r="B24" s="2">
-        <v>-85.2453</v>
+        <v>-85.105599999999995</v>
       </c>
       <c r="C24" s="2">
-        <v>286.71159999999998</v>
+        <v>289.40949999999998</v>
       </c>
       <c r="D24" s="2">
-        <v>0.55389999999999995</v>
+        <v>1.0407999999999999</v>
       </c>
       <c r="E24" s="2">
-        <v>311327.16330000001</v>
+        <v>311327.1053</v>
       </c>
       <c r="F24" s="2">
-        <v>8807897.4686999992</v>
+        <v>8807897.6717000008</v>
       </c>
       <c r="G24" s="2">
-        <v>3993.6318999999999</v>
+        <v>3993.6406000000002</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1487,22 +1487,22 @@
         <v>210</v>
       </c>
       <c r="B25" s="2">
-        <v>-84.911699999999996</v>
+        <v>-84.651200000000003</v>
       </c>
       <c r="C25" s="2">
-        <v>301.96499999999997</v>
+        <v>304.40530000000001</v>
       </c>
       <c r="D25" s="2">
-        <v>4.0381</v>
+        <v>4.2266000000000004</v>
       </c>
       <c r="E25" s="2">
-        <v>311326.39020000002</v>
+        <v>311326.31839999999</v>
       </c>
       <c r="F25" s="2">
-        <v>8807897.8226999994</v>
+        <v>8807898.0767999999</v>
       </c>
       <c r="G25" s="2">
-        <v>3983.6687999999999</v>
+        <v>3983.6806000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1510,22 +1510,22 @@
         <v>220</v>
       </c>
       <c r="B26" s="2">
-        <v>-82.824700000000007</v>
+        <v>-82.319400000000002</v>
       </c>
       <c r="C26" s="2">
-        <v>316.42899999999997</v>
+        <v>321.20850000000002</v>
       </c>
       <c r="D26" s="2">
-        <v>7.7430000000000003</v>
+        <v>8.9654000000000007</v>
       </c>
       <c r="E26" s="2">
-        <v>311325.58350000001</v>
+        <v>311325.51520000002</v>
       </c>
       <c r="F26" s="2">
-        <v>8807898.5098999999</v>
+        <v>8807898.8609999996</v>
       </c>
       <c r="G26" s="2">
-        <v>3973.7276999999999</v>
+        <v>3973.7473</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1533,22 +1533,22 @@
         <v>230</v>
       </c>
       <c r="B27" s="2">
-        <v>-82.105900000000005</v>
+        <v>-81.917299999999997</v>
       </c>
       <c r="C27" s="2">
-        <v>324.44709999999998</v>
+        <v>324.15410000000003</v>
       </c>
       <c r="D27" s="2">
-        <v>3.8157000000000001</v>
+        <v>1.7094</v>
       </c>
       <c r="E27" s="2">
-        <v>311324.7537</v>
+        <v>311324.68479999999</v>
       </c>
       <c r="F27" s="2">
-        <v>8807899.5210999995</v>
+        <v>8807899.9517999999</v>
       </c>
       <c r="G27" s="2">
-        <v>3963.8141999999998</v>
+        <v>3963.8418000000001</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1556,22 +1556,22 @@
         <v>240</v>
       </c>
       <c r="B28" s="2">
-        <v>-82.064599999999999</v>
+        <v>-81.987499999999997</v>
       </c>
       <c r="C28" s="2">
-        <v>323.13720000000001</v>
+        <v>324.08159999999998</v>
       </c>
       <c r="D28" s="2">
-        <v>0.55510000000000004</v>
+        <v>0.21260000000000001</v>
       </c>
       <c r="E28" s="2">
-        <v>311323.94040000002</v>
+        <v>311323.86430000002</v>
       </c>
       <c r="F28" s="2">
-        <v>8807900.6320999991</v>
+        <v>8807901.0859999992</v>
       </c>
       <c r="G28" s="2">
-        <v>3953.9095000000002</v>
+        <v>3953.9403000000002</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1579,22 +1579,22 @@
         <v>250</v>
       </c>
       <c r="B29" s="2">
-        <v>-82.078400000000002</v>
+        <v>-81.983999999999995</v>
       </c>
       <c r="C29" s="2">
-        <v>323.07049999999998</v>
+        <v>324.05900000000003</v>
       </c>
       <c r="D29" s="2">
-        <v>4.9599999999999998E-2</v>
+        <v>1.41E-2</v>
       </c>
       <c r="E29" s="2">
-        <v>311323.11219999997</v>
+        <v>311323.04619999998</v>
       </c>
       <c r="F29" s="2">
-        <v>8807901.7352000009</v>
+        <v>8807902.2149999999</v>
       </c>
       <c r="G29" s="2">
-        <v>3944.0050999999999</v>
+        <v>3944.0378999999998</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1602,22 +1602,22 @@
         <v>260</v>
       </c>
       <c r="B30" s="2">
-        <v>-81.900499999999994</v>
+        <v>-81.816699999999997</v>
       </c>
       <c r="C30" s="2">
-        <v>322.21949999999998</v>
+        <v>323.90390000000002</v>
       </c>
       <c r="D30" s="2">
-        <v>0.64129999999999998</v>
+        <v>0.50629999999999997</v>
       </c>
       <c r="E30" s="2">
-        <v>311322.26659999997</v>
+        <v>311322.21759999997</v>
       </c>
       <c r="F30" s="2">
-        <v>8807902.8428000007</v>
+        <v>8807903.3545999993</v>
       </c>
       <c r="G30" s="2">
-        <v>3934.1026000000002</v>
+        <v>3934.1377000000002</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1625,22 +1625,22 @@
         <v>270</v>
       </c>
       <c r="B31" s="2">
-        <v>-81.974000000000004</v>
+        <v>-81.884299999999996</v>
       </c>
       <c r="C31" s="2">
-        <v>323.1961</v>
+        <v>324.38069999999999</v>
       </c>
       <c r="D31" s="2">
-        <v>0.46629999999999999</v>
+        <v>0.28689999999999999</v>
       </c>
       <c r="E31" s="2">
-        <v>311321.41680000001</v>
+        <v>311321.3872</v>
       </c>
       <c r="F31" s="2">
-        <v>8807903.9585999995</v>
+        <v>8807904.5033999998</v>
       </c>
       <c r="G31" s="2">
-        <v>3924.2015000000001</v>
+        <v>3924.2386999999999</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1648,22 +1648,22 @@
         <v>280</v>
       </c>
       <c r="B32" s="2">
-        <v>-81.885400000000004</v>
+        <v>-81.869699999999995</v>
       </c>
       <c r="C32" s="2">
-        <v>324.10950000000003</v>
+        <v>325.65249999999997</v>
       </c>
       <c r="D32" s="2">
-        <v>0.46750000000000003</v>
+        <v>0.54090000000000005</v>
       </c>
       <c r="E32" s="2">
-        <v>311320.58480000001</v>
+        <v>311320.5772</v>
       </c>
       <c r="F32" s="2">
-        <v>8807905.0892999992</v>
+        <v>8807905.6611000001</v>
       </c>
       <c r="G32" s="2">
-        <v>3914.3004999999998</v>
+        <v>3914.3389999999999</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1671,22 +1671,22 @@
         <v>290</v>
       </c>
       <c r="B33" s="2">
-        <v>-83.944299999999998</v>
+        <v>-84.216499999999996</v>
       </c>
       <c r="C33" s="2">
-        <v>328.89640000000003</v>
+        <v>332.798</v>
       </c>
       <c r="D33" s="2">
-        <v>6.4202000000000004</v>
+        <v>7.4905999999999997</v>
       </c>
       <c r="E33" s="2">
-        <v>311319.89860000001</v>
+        <v>311319.94790000003</v>
       </c>
       <c r="F33" s="2">
-        <v>8807906.1127000004</v>
+        <v>8807906.693</v>
       </c>
       <c r="G33" s="2">
-        <v>3904.3784999999998</v>
+        <v>3904.4146999999998</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1694,22 +1694,22 @@
         <v>300</v>
       </c>
       <c r="B34" s="2">
-        <v>-85.167599999999993</v>
+        <v>-85.281400000000005</v>
       </c>
       <c r="C34" s="2">
-        <v>353.94330000000002</v>
+        <v>356.74310000000003</v>
       </c>
       <c r="D34" s="2">
-        <v>7.9287000000000001</v>
+        <v>7.2369000000000003</v>
       </c>
       <c r="E34" s="2">
-        <v>311319.58169999998</v>
+        <v>311319.69420000003</v>
       </c>
       <c r="F34" s="2">
-        <v>8807906.9832000006</v>
+        <v>8807907.5517999995</v>
       </c>
       <c r="G34" s="2">
-        <v>3894.4241999999999</v>
+        <v>3894.4571000000001</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1717,22 +1717,22 @@
         <v>310</v>
       </c>
       <c r="B35" s="2">
-        <v>-85.489000000000004</v>
+        <v>-85.478800000000007</v>
       </c>
       <c r="C35" s="2">
-        <v>354.81610000000001</v>
+        <v>358.87470000000002</v>
       </c>
       <c r="D35" s="2">
-        <v>0.98760000000000003</v>
+        <v>0.78480000000000005</v>
       </c>
       <c r="E35" s="2">
-        <v>311319.50170000002</v>
+        <v>311319.66310000001</v>
       </c>
       <c r="F35" s="2">
-        <v>8807907.7937000003</v>
+        <v>8807908.3564999998</v>
       </c>
       <c r="G35" s="2">
-        <v>3884.4573999999998</v>
+        <v>3884.4895999999999</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -1740,22 +1740,22 @@
         <v>320</v>
       </c>
       <c r="B36" s="2">
-        <v>-85.396900000000002</v>
+        <v>-85.236400000000003</v>
       </c>
       <c r="C36" s="2">
-        <v>356.3897</v>
+        <v>3.9E-2</v>
       </c>
       <c r="D36" s="2">
-        <v>0.46589999999999998</v>
+        <v>0.78029999999999999</v>
       </c>
       <c r="E36" s="2">
-        <v>311319.44089999999</v>
+        <v>311319.6556</v>
       </c>
       <c r="F36" s="2">
-        <v>8807908.5857999995</v>
+        <v>8807909.1657999996</v>
       </c>
       <c r="G36" s="2">
-        <v>3874.4890999999998</v>
+        <v>3874.5225</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -1763,22 +1763,22 @@
         <v>330</v>
       </c>
       <c r="B37" s="2">
-        <v>-85.412899999999993</v>
+        <v>-85.293800000000005</v>
       </c>
       <c r="C37" s="2">
-        <v>356.12990000000002</v>
+        <v>359.5573</v>
       </c>
       <c r="D37" s="2">
-        <v>7.8700000000000006E-2</v>
+        <v>0.20949999999999999</v>
       </c>
       <c r="E37" s="2">
-        <v>311319.38860000001</v>
+        <v>311319.65269999998</v>
       </c>
       <c r="F37" s="2">
-        <v>8807909.3852999993</v>
+        <v>8807909.9912</v>
       </c>
       <c r="G37" s="2">
-        <v>3864.5212000000001</v>
+        <v>3864.5565999999999</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1786,22 +1786,22 @@
         <v>340</v>
       </c>
       <c r="B38" s="2">
-        <v>-85.285200000000003</v>
+        <v>-85.385000000000005</v>
       </c>
       <c r="C38" s="2">
-        <v>355.18509999999998</v>
+        <v>357.97629999999998</v>
       </c>
       <c r="D38" s="2">
-        <v>0.4466</v>
+        <v>0.47270000000000001</v>
       </c>
       <c r="E38" s="2">
-        <v>311319.3272</v>
+        <v>311319.63540000003</v>
       </c>
       <c r="F38" s="2">
-        <v>8807910.1938000005</v>
+        <v>8807910.8035000004</v>
       </c>
       <c r="G38" s="2">
-        <v>3854.5540999999998</v>
+        <v>3854.5897</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1809,22 +1809,22 @@
         <v>350</v>
       </c>
       <c r="B39" s="2">
-        <v>-85.580399999999997</v>
+        <v>-85.727199999999996</v>
       </c>
       <c r="C39" s="2">
-        <v>351.60910000000001</v>
+        <v>355.4855</v>
       </c>
       <c r="D39" s="2">
-        <v>1.2301</v>
+        <v>1.1782999999999999</v>
       </c>
       <c r="E39" s="2">
-        <v>311319.23639999999</v>
+        <v>311319.59179999999</v>
       </c>
       <c r="F39" s="2">
-        <v>8807910.9845000003</v>
+        <v>8807911.5768999998</v>
       </c>
       <c r="G39" s="2">
-        <v>3844.5859</v>
+        <v>3844.6197999999999</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -1832,22 +1832,22 @@
         <v>360</v>
       </c>
       <c r="B40" s="2">
-        <v>-85.974199999999996</v>
+        <v>-86.015500000000003</v>
       </c>
       <c r="C40" s="2">
-        <v>349.51130000000001</v>
+        <v>353.64580000000001</v>
       </c>
       <c r="D40" s="2">
-        <v>1.2687999999999999</v>
+        <v>0.95169999999999999</v>
       </c>
       <c r="E40" s="2">
-        <v>311319.11629999999</v>
+        <v>311319.52409999998</v>
       </c>
       <c r="F40" s="2">
-        <v>8807911.7107999995</v>
+        <v>8807912.2936000004</v>
       </c>
       <c r="G40" s="2">
-        <v>3834.6131</v>
+        <v>3834.6457</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -1855,22 +1855,22 @@
         <v>370</v>
       </c>
       <c r="B41" s="2">
-        <v>-86.259799999999998</v>
+        <v>-86.300700000000006</v>
       </c>
       <c r="C41" s="2">
-        <v>348.41</v>
+        <v>353.83339999999998</v>
       </c>
       <c r="D41" s="2">
-        <v>0.88549999999999995</v>
+        <v>0.85660000000000003</v>
       </c>
       <c r="E41" s="2">
-        <v>311318.98690000002</v>
+        <v>311319.4509</v>
       </c>
       <c r="F41" s="2">
-        <v>8807912.3754999992</v>
+        <v>8807912.9595999997</v>
       </c>
       <c r="G41" s="2">
-        <v>3824.6361000000002</v>
+        <v>3824.6682000000001</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -1878,22 +1878,22 @@
         <v>380</v>
       </c>
       <c r="B42" s="2">
-        <v>-86.684299999999993</v>
+        <v>-86.6678</v>
       </c>
       <c r="C42" s="2">
-        <v>350.34750000000003</v>
+        <v>356.39789999999999</v>
       </c>
       <c r="D42" s="2">
-        <v>1.3227</v>
+        <v>1.1977</v>
       </c>
       <c r="E42" s="2">
-        <v>311318.87290000002</v>
+        <v>311319.39799999999</v>
       </c>
       <c r="F42" s="2">
-        <v>8807912.9801000003</v>
+        <v>8807913.5703999996</v>
       </c>
       <c r="G42" s="2">
-        <v>3814.6550999999999</v>
+        <v>3814.6871000000001</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -1901,22 +1901,22 @@
         <v>390</v>
       </c>
       <c r="B43" s="2">
-        <v>-86.644000000000005</v>
+        <v>-86.509399999999999</v>
       </c>
       <c r="C43" s="2">
-        <v>350.92779999999999</v>
+        <v>355.02269999999999</v>
       </c>
       <c r="D43" s="2">
-        <v>0.1578</v>
+        <v>0.53480000000000005</v>
       </c>
       <c r="E43" s="2">
-        <v>311318.7782</v>
+        <v>311319.35340000002</v>
       </c>
       <c r="F43" s="2">
-        <v>8807913.5541999992</v>
+        <v>8807914.1636999995</v>
       </c>
       <c r="G43" s="2">
-        <v>3804.6720999999998</v>
+        <v>3804.7048</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -1924,22 +1924,22 @@
         <v>400</v>
       </c>
       <c r="B44" s="2">
-        <v>-86.688199999999995</v>
+        <v>-86.605699999999999</v>
       </c>
       <c r="C44" s="2">
-        <v>350.02730000000003</v>
+        <v>356.94619999999998</v>
       </c>
       <c r="D44" s="2">
-        <v>0.2056</v>
+        <v>0.4511</v>
       </c>
       <c r="E44" s="2">
-        <v>311318.68199999997</v>
+        <v>311319.3112</v>
       </c>
       <c r="F44" s="2">
-        <v>8807914.1276999991</v>
+        <v>8807914.7625999991</v>
       </c>
       <c r="G44" s="2">
-        <v>3794.6889999999999</v>
+        <v>3794.7229000000002</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -1947,22 +1947,22 @@
         <v>410</v>
       </c>
       <c r="B45" s="2">
-        <v>-86.6327</v>
+        <v>-86.590500000000006</v>
       </c>
       <c r="C45" s="2">
-        <v>350.36059999999998</v>
+        <v>357.54899999999998</v>
       </c>
       <c r="D45" s="2">
-        <v>0.1764</v>
+        <v>0.1166</v>
       </c>
       <c r="E45" s="2">
-        <v>311318.58279999997</v>
+        <v>311319.28269999998</v>
       </c>
       <c r="F45" s="2">
-        <v>8807914.7017999999</v>
+        <v>8807915.3552999999</v>
       </c>
       <c r="G45" s="2">
-        <v>3784.7060000000001</v>
+        <v>3784.7404999999999</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -1970,22 +1970,22 @@
         <v>420</v>
       </c>
       <c r="B46" s="2">
-        <v>-86.703999999999994</v>
+        <v>-86.798100000000005</v>
       </c>
       <c r="C46" s="2">
-        <v>349.94400000000002</v>
+        <v>359.01690000000002</v>
       </c>
       <c r="D46" s="2">
-        <v>0.22589999999999999</v>
+        <v>0.67249999999999999</v>
       </c>
       <c r="E46" s="2">
-        <v>311318.48349999997</v>
+        <v>311319.26520000002</v>
       </c>
       <c r="F46" s="2">
-        <v>8807915.2743999995</v>
+        <v>8807915.9316000007</v>
       </c>
       <c r="G46" s="2">
-        <v>3774.7229000000002</v>
+        <v>3774.7572</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -1993,22 +1993,22 @@
         <v>430</v>
       </c>
       <c r="B47" s="2">
-        <v>-86.727900000000005</v>
+        <v>-86.8125</v>
       </c>
       <c r="C47" s="2">
-        <v>348.5693</v>
+        <v>358.81349999999998</v>
       </c>
       <c r="D47" s="2">
-        <v>0.24690000000000001</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E47" s="2">
-        <v>311318.37670000002</v>
+        <v>311319.25459999999</v>
       </c>
       <c r="F47" s="2">
-        <v>8807915.8370999992</v>
+        <v>8807916.4888000004</v>
       </c>
       <c r="G47" s="2">
-        <v>3764.7393000000002</v>
+        <v>3764.7727</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2016,22 +2016,22 @@
         <v>440</v>
       </c>
       <c r="B48" s="2">
-        <v>-86.87</v>
+        <v>-86.752600000000001</v>
       </c>
       <c r="C48" s="2">
-        <v>346.32369999999997</v>
+        <v>355.2989</v>
       </c>
       <c r="D48" s="2">
-        <v>0.56840000000000002</v>
+        <v>0.61829999999999996</v>
       </c>
       <c r="E48" s="2">
-        <v>311318.25559999997</v>
+        <v>311319.22570000001</v>
       </c>
       <c r="F48" s="2">
-        <v>8807916.3820999991</v>
+        <v>8807917.0491000004</v>
       </c>
       <c r="G48" s="2">
-        <v>3754.7548999999999</v>
+        <v>3754.7885000000001</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2039,22 +2039,22 @@
         <v>450</v>
       </c>
       <c r="B49" s="2">
-        <v>-86.825400000000002</v>
+        <v>-86.624799999999993</v>
       </c>
       <c r="C49" s="2">
-        <v>347.03640000000001</v>
+        <v>354.3537</v>
       </c>
       <c r="D49" s="2">
-        <v>0.17799999999999999</v>
+        <v>0.41689999999999999</v>
       </c>
       <c r="E49" s="2">
-        <v>311318.12890000001</v>
+        <v>311319.17349999998</v>
       </c>
       <c r="F49" s="2">
-        <v>8807916.9171999991</v>
+        <v>8807917.6242999993</v>
       </c>
       <c r="G49" s="2">
-        <v>3744.77</v>
+        <v>3744.8051999999998</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2062,22 +2062,22 @@
         <v>460</v>
       </c>
       <c r="B50" s="2">
-        <v>-86.765100000000004</v>
+        <v>-86.716700000000003</v>
       </c>
       <c r="C50" s="2">
-        <v>344.08969999999999</v>
+        <v>355.28750000000002</v>
       </c>
       <c r="D50" s="2">
-        <v>0.5262</v>
+        <v>0.32</v>
       </c>
       <c r="E50" s="2">
-        <v>311317.98950000003</v>
+        <v>311319.12099999998</v>
       </c>
       <c r="F50" s="2">
-        <v>8807917.4583999999</v>
+        <v>8807918.2026000004</v>
       </c>
       <c r="G50" s="2">
-        <v>3734.7856999999999</v>
+        <v>3734.8220999999999</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -2085,22 +2085,22 @@
         <v>470</v>
       </c>
       <c r="B51" s="2">
-        <v>-86.935699999999997</v>
+        <v>-86.9114</v>
       </c>
       <c r="C51" s="2">
-        <v>342.06009999999998</v>
+        <v>355.14269999999999</v>
       </c>
       <c r="D51" s="2">
-        <v>0.61140000000000005</v>
+        <v>0.58460000000000001</v>
       </c>
       <c r="E51" s="2">
-        <v>311317.82980000001</v>
+        <v>311319.0747</v>
       </c>
       <c r="F51" s="2">
-        <v>8807917.9839999992</v>
+        <v>8807918.7564000003</v>
       </c>
       <c r="G51" s="2">
-        <v>3724.8008</v>
+        <v>3724.8375000000001</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2108,22 +2108,22 @@
         <v>480</v>
       </c>
       <c r="B52" s="2">
-        <v>-86.989199999999997</v>
+        <v>-87.084400000000002</v>
       </c>
       <c r="C52" s="2">
-        <v>343.61649999999997</v>
+        <v>354.17989999999998</v>
       </c>
       <c r="D52" s="2">
-        <v>0.2949</v>
+        <v>0.54059999999999997</v>
       </c>
       <c r="E52" s="2">
-        <v>311317.67340000003</v>
+        <v>311319.02610000002</v>
       </c>
       <c r="F52" s="2">
-        <v>8807918.4902999997</v>
+        <v>8807919.2778999992</v>
       </c>
       <c r="G52" s="2">
-        <v>3714.8148999999999</v>
+        <v>3714.8512999999998</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -2131,22 +2131,22 @@
         <v>490</v>
       </c>
       <c r="B53" s="2">
-        <v>-87.1053</v>
+        <v>-87.079099999999997</v>
       </c>
       <c r="C53" s="2">
-        <v>338.88010000000003</v>
+        <v>349.74650000000003</v>
       </c>
       <c r="D53" s="2">
-        <v>0.81020000000000003</v>
+        <v>0.67710000000000004</v>
       </c>
       <c r="E53" s="2">
-        <v>311317.50829999999</v>
+        <v>311318.95490000001</v>
       </c>
       <c r="F53" s="2">
-        <v>8807918.9778000005</v>
+        <v>8807919.7816000003</v>
       </c>
       <c r="G53" s="2">
-        <v>3704.8281000000002</v>
+        <v>3704.8642</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -2154,22 +2154,22 @@
         <v>500</v>
       </c>
       <c r="B54" s="2">
-        <v>-87.325199999999995</v>
+        <v>-87.153700000000001</v>
       </c>
       <c r="C54" s="2">
-        <v>336.14600000000002</v>
+        <v>349.44499999999999</v>
       </c>
       <c r="D54" s="2">
-        <v>0.77070000000000005</v>
+        <v>0.2283</v>
       </c>
       <c r="E54" s="2">
-        <v>311317.32299999997</v>
+        <v>311318.86410000001</v>
       </c>
       <c r="F54" s="2">
-        <v>8807919.4266999997</v>
+        <v>8807920.2763999999</v>
       </c>
       <c r="G54" s="2">
-        <v>3694.84</v>
+        <v>3694.8769000000002</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -2177,22 +2177,22 @@
         <v>510</v>
       </c>
       <c r="B55" s="2">
-        <v>-87.25</v>
+        <v>-87.228499999999997</v>
       </c>
       <c r="C55" s="2">
-        <v>334.34179999999998</v>
+        <v>348.846</v>
       </c>
       <c r="D55" s="2">
-        <v>0.34129999999999999</v>
+        <v>0.24110000000000001</v>
       </c>
       <c r="E55" s="2">
-        <v>311317.12479999999</v>
+        <v>311318.77179999999</v>
       </c>
       <c r="F55" s="2">
-        <v>8807919.8563999999</v>
+        <v>8807920.7577</v>
       </c>
       <c r="G55" s="2">
-        <v>3684.8512000000001</v>
+        <v>3684.8888999999999</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -2200,22 +2200,22 @@
         <v>520</v>
       </c>
       <c r="B56" s="2">
-        <v>-87.162899999999993</v>
+        <v>-87.1965</v>
       </c>
       <c r="C56" s="2">
-        <v>332.9162</v>
+        <v>348.20510000000002</v>
       </c>
       <c r="D56" s="2">
-        <v>0.33439999999999998</v>
+        <v>0.1341</v>
       </c>
       <c r="E56" s="2">
-        <v>311316.90820000001</v>
+        <v>311318.67509999999</v>
       </c>
       <c r="F56" s="2">
-        <v>8807920.2928999998</v>
+        <v>8807921.2343000006</v>
       </c>
       <c r="G56" s="2">
-        <v>3674.8631</v>
+        <v>3674.9007000000001</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -2223,22 +2223,22 @@
         <v>530</v>
       </c>
       <c r="B57" s="2">
-        <v>-87.189099999999996</v>
+        <v>-87.034499999999994</v>
       </c>
       <c r="C57" s="2">
-        <v>333.27050000000003</v>
+        <v>351.21859999999998</v>
       </c>
       <c r="D57" s="2">
-        <v>9.4600000000000004E-2</v>
+        <v>0.66539999999999999</v>
       </c>
       <c r="E57" s="2">
-        <v>311316.68530000001</v>
+        <v>311318.58559999999</v>
       </c>
       <c r="F57" s="2">
-        <v>8807920.7323000003</v>
+        <v>8807921.7292999998</v>
       </c>
       <c r="G57" s="2">
-        <v>3664.8751999999999</v>
+        <v>3664.9133999999999</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -2246,22 +2246,22 @@
         <v>540</v>
       </c>
       <c r="B58" s="2">
-        <v>-87.294700000000006</v>
+        <v>-87.1691</v>
       </c>
       <c r="C58" s="2">
-        <v>331.42140000000001</v>
+        <v>349.24630000000002</v>
       </c>
       <c r="D58" s="2">
-        <v>0.41410000000000002</v>
+        <v>0.50249999999999995</v>
       </c>
       <c r="E58" s="2">
-        <v>311316.4621</v>
+        <v>311318.5</v>
       </c>
       <c r="F58" s="2">
-        <v>8807921.1585000008</v>
+        <v>8807922.2276000008</v>
       </c>
       <c r="G58" s="2">
-        <v>3654.8868000000002</v>
+        <v>3654.9261999999999</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -2269,22 +2269,22 @@
         <v>550</v>
       </c>
       <c r="B59" s="2">
-        <v>-87.051699999999997</v>
+        <v>-87.151399999999995</v>
       </c>
       <c r="C59" s="2">
-        <v>335.41669999999999</v>
+        <v>351.07830000000001</v>
       </c>
       <c r="D59" s="2">
-        <v>0.93810000000000004</v>
+        <v>0.27739999999999998</v>
       </c>
       <c r="E59" s="2">
-        <v>311316.24219999998</v>
+        <v>311318.4154</v>
       </c>
       <c r="F59" s="2">
-        <v>8807921.5996000003</v>
+        <v>8807922.7157000005</v>
       </c>
       <c r="G59" s="2">
-        <v>3644.8989999999999</v>
+        <v>3644.9385000000002</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -2292,22 +2292,22 @@
         <v>560</v>
       </c>
       <c r="B60" s="2">
-        <v>-86.987799999999993</v>
+        <v>-87.012799999999999</v>
       </c>
       <c r="C60" s="2">
-        <v>333.28649999999999</v>
+        <v>349.47219999999999</v>
       </c>
       <c r="D60" s="2">
-        <v>0.3836</v>
+        <v>0.48259999999999997</v>
       </c>
       <c r="E60" s="2">
-        <v>311316.0171</v>
+        <v>311318.32929999998</v>
       </c>
       <c r="F60" s="2">
-        <v>8807922.0681999996</v>
+        <v>8807923.2172999997</v>
       </c>
       <c r="G60" s="2">
-        <v>3634.9124999999999</v>
+        <v>3634.9515000000001</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -2315,22 +2315,22 @@
         <v>570</v>
       </c>
       <c r="B61" s="2">
-        <v>-86.924899999999994</v>
+        <v>-87.131900000000002</v>
       </c>
       <c r="C61" s="2">
-        <v>333.56009999999998</v>
+        <v>351.51010000000002</v>
       </c>
       <c r="D61" s="2">
-        <v>0.19370000000000001</v>
+        <v>0.47449999999999998</v>
       </c>
       <c r="E61" s="2">
-        <v>311315.77960000001</v>
+        <v>311318.24469999998</v>
       </c>
       <c r="F61" s="2">
-        <v>8807922.5430999994</v>
+        <v>8807923.7208999991</v>
       </c>
       <c r="G61" s="2">
-        <v>3624.9265999999998</v>
+        <v>3624.9645</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -2338,22 +2338,22 @@
         <v>580</v>
       </c>
       <c r="B62" s="2">
-        <v>-87.017700000000005</v>
+        <v>-87.128399999999999</v>
       </c>
       <c r="C62" s="2">
-        <v>337.09199999999998</v>
+        <v>355.50920000000002</v>
       </c>
       <c r="D62" s="2">
-        <v>0.62519999999999998</v>
+        <v>0.60060000000000002</v>
       </c>
       <c r="E62" s="2">
-        <v>311315.5589</v>
+        <v>311318.18819999998</v>
       </c>
       <c r="F62" s="2">
-        <v>8807923.0229000002</v>
+        <v>8807924.2181000002</v>
       </c>
       <c r="G62" s="2">
-        <v>3614.9405999999999</v>
+        <v>3614.9771000000001</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -2361,22 +2361,22 @@
         <v>590</v>
       </c>
       <c r="B63" s="2">
-        <v>-87.096699999999998</v>
+        <v>-87.213999999999999</v>
       </c>
       <c r="C63" s="2">
-        <v>334.24369999999999</v>
+        <v>353.03660000000002</v>
       </c>
       <c r="D63" s="2">
-        <v>0.4985</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="E63" s="2">
-        <v>311315.34759999998</v>
+        <v>311318.13909999997</v>
       </c>
       <c r="F63" s="2">
-        <v>8807923.4905999992</v>
+        <v>8807924.7090000007</v>
       </c>
       <c r="G63" s="2">
-        <v>3604.9537999999998</v>
+        <v>3604.9893000000002</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -2384,22 +2384,22 @@
         <v>600</v>
       </c>
       <c r="B64" s="2">
-        <v>-87.047300000000007</v>
+        <v>-86.848600000000005</v>
       </c>
       <c r="C64" s="2">
-        <v>332.92059999999998</v>
+        <v>352.82339999999999</v>
       </c>
       <c r="D64" s="2">
-        <v>0.251</v>
+        <v>1.0968</v>
       </c>
       <c r="E64" s="2">
-        <v>311315.12030000001</v>
+        <v>311318.07530000003</v>
       </c>
       <c r="F64" s="2">
-        <v>8807923.9480000008</v>
+        <v>8807925.2229999993</v>
       </c>
       <c r="G64" s="2">
-        <v>3594.9668000000001</v>
+        <v>3595.0027</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2407,22 +2407,68 @@
         <v>610</v>
       </c>
       <c r="B65" s="2">
-        <v>-86.981399999999994</v>
+        <v>-86.887900000000002</v>
       </c>
       <c r="C65" s="2">
-        <v>332.4855</v>
+        <v>352.8449</v>
       </c>
       <c r="D65" s="2">
-        <v>0.2092</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="E65" s="2">
-        <v>311314.88140000001</v>
+        <v>311318.00719999999</v>
       </c>
       <c r="F65" s="2">
-        <v>8807924.4108000007</v>
+        <v>8807925.7651000004</v>
       </c>
       <c r="G65" s="2">
-        <v>3584.9803999999999</v>
+        <v>3585.0176999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>620</v>
+      </c>
+      <c r="B66" s="2">
+        <v>-86.991100000000003</v>
+      </c>
+      <c r="C66" s="2">
+        <v>353.04739999999998</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0.3115</v>
+      </c>
+      <c r="E66" s="2">
+        <v>311317.94160000002</v>
+      </c>
+      <c r="F66" s="2">
+        <v>8807926.2949000001</v>
+      </c>
+      <c r="G66" s="2">
+        <v>3575.0319</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>630</v>
+      </c>
+      <c r="B67" s="2">
+        <v>-86.808800000000005</v>
+      </c>
+      <c r="C67" s="2">
+        <v>352.70490000000001</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.54969999999999997</v>
+      </c>
+      <c r="E67" s="2">
+        <v>311317.87449999998</v>
+      </c>
+      <c r="F67" s="2">
+        <v>8807926.8314999994</v>
+      </c>
+      <c r="G67" s="2">
+        <v>3565.0466000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2431,5 +2477,6 @@
     <mergeCell ref="C1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>